<commit_message>
back-end signup send mail
</commit_message>
<xml_diff>
--- a/Document/Issues-Report_GROUP2.xlsx
+++ b/Document/Issues-Report_GROUP2.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoàng\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Septemple_5\SWP391\homeSangTroKhang\SWP391-OnlineLearn\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37D01955-1804-407A-A72E-2184ED206CA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1F029D15-4B34-8B4D-AA03-001B4FC8F913}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12450"/>
   </bookViews>
   <sheets>
     <sheet name="Issues Report" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
   <si>
     <t>Title</t>
   </si>
@@ -60,15 +59,9 @@
     <t>Functions/Screens</t>
   </si>
   <si>
-    <t>iter2</t>
-  </si>
-  <si>
     <t xml:space="preserve">When member pull code from github to their pc because they have same name variables and class </t>
   </si>
   <si>
-    <t>Conflict</t>
-  </si>
-  <si>
     <t>Error file not found</t>
   </si>
   <si>
@@ -105,18 +98,12 @@
     <t>23/2/2023</t>
   </si>
   <si>
-    <t>iter3</t>
-  </si>
-  <si>
     <t>user profile</t>
   </si>
   <si>
     <t>24/2/2023</t>
   </si>
   <si>
-    <t>inter3</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -127,17 +114,68 @@
   </si>
   <si>
     <t xml:space="preserve">add lib local </t>
+  </si>
+  <si>
+    <t>Kiên</t>
+  </si>
+  <si>
+    <t>25/2/2023</t>
+  </si>
+  <si>
+    <t>Can connect to database</t>
+  </si>
+  <si>
+    <t>wrong username and password</t>
+  </si>
+  <si>
+    <t>26/2/2023</t>
+  </si>
+  <si>
+    <t>Error creating an account in the database when the account registration has not been completed</t>
+  </si>
+  <si>
+    <t>Error account creation error</t>
+  </si>
+  <si>
+    <t>can't go to another page</t>
+  </si>
+  <si>
+    <t>wrong link</t>
+  </si>
+  <si>
+    <t>Can't run project</t>
+  </si>
+  <si>
+    <t>Error in web.xml</t>
+  </si>
+  <si>
+    <t>27/2/2023</t>
+  </si>
+  <si>
+    <t>inter 3</t>
+  </si>
+  <si>
+    <t>Error in project.xml</t>
+  </si>
+  <si>
+    <t>28/2/2023</t>
+  </si>
+  <si>
+    <t>iter 3</t>
+  </si>
+  <si>
+    <t>iter 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -203,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -226,6 +264,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,26 +581,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5B9144B-93AC-0243-B48F-1FC49AC75151}">
-  <dimension ref="A1:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.36328125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="45" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.36328125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="39.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.90625" style="3"/>
-    <col min="7" max="8" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="3"/>
-    <col min="10" max="10" width="15.36328125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.90625" style="3"/>
+    <col min="1" max="1" width="27.375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="83.375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="39.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.875" style="3"/>
+    <col min="7" max="8" width="10.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="3"/>
+    <col min="10" max="10" width="15.375" style="3" customWidth="1"/>
+    <col min="11" max="11" width="16.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -598,11 +639,9 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="43.5" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>13</v>
-      </c>
+      <c r="A2" s="5"/>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -610,16 +649,16 @@
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" s="6">
         <v>45048</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
@@ -629,7 +668,7 @@
         <v>404</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C3" s="4">
         <v>2</v>
@@ -637,16 +676,16 @@
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G3" s="6">
         <v>45140</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -656,7 +695,7 @@
         <v>500</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4">
         <v>3</v>
@@ -664,96 +703,339 @@
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G4" s="6">
         <v>45201</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" s="4">
         <v>4</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="I5" s="4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:11">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4">
         <v>5</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-      <c r="I7" s="4"/>
+      <c r="I7" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="8">
+        <v>404</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="4">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11" s="9">
+        <v>44929</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="9">
+        <v>44929</v>
+      </c>
+      <c r="H12" s="9">
+        <v>44988</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+    </row>
+    <row r="17" spans="1:11">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+    </row>
+    <row r="18" spans="1:11">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>